<commit_message>
redid OXY values, may using july calibrator (check notebook 1/30./2023)
made new spreadsheet (master) with _OXYredo after it as I didn't want to change the original sheets. OXY is redid in that one (oxy, oxystd, and oi)

made changes to CV due to OXY
</commit_message>
<xml_diff>
--- a/output/Inter_IntraVariation_CK.xlsx
+++ b/output/Inter_IntraVariation_CK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive - USU\Desktop\ASU green iguana 2021\greeniguanaAnalysis\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABB3C95-8834-42F0-9E8E-FE08416B4680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2412CD08-AB4F-4AAA-AF99-59BD37222774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="270" windowWidth="25440" windowHeight="15270" xr2:uid="{4E0824B5-875B-40B9-920C-3369E689C253}"/>
   </bookViews>
@@ -274,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -309,6 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,12 +624,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD948F92-F30E-4C35-9CD4-36F7688BAFFD}">
-  <dimension ref="A1:R510"/>
+  <dimension ref="A1:Z510"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1:Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,9 +643,10 @@
     <col min="12" max="12" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.1796875" style="25"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -695,8 +697,16 @@
         <v>8</v>
       </c>
       <c r="R1" s="26"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S1" s="9"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="11"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -749,8 +759,16 @@
         <f>_xlfn.STDEV.S(N2:O2,N8:O13)/AVERAGE(N2:O2, N8:O13)*100</f>
         <v>23.205847675789411</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S2" s="13"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="30"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
@@ -789,8 +807,12 @@
       </c>
       <c r="P3" s="20"/>
       <c r="Q3" s="7"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S3" s="12"/>
+      <c r="U3" s="1"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="7"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
@@ -829,8 +851,12 @@
       </c>
       <c r="P4" s="20"/>
       <c r="Q4" s="7"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S4" s="12"/>
+      <c r="U4" s="1"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="7"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -870,8 +896,12 @@
       </c>
       <c r="P5" s="20"/>
       <c r="Q5" s="7"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S5" s="12"/>
+      <c r="U5" s="1"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="7"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
@@ -914,8 +944,12 @@
       </c>
       <c r="P6" s="23"/>
       <c r="Q6" s="8"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S6" s="12"/>
+      <c r="U6" s="1"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="7"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -957,8 +991,12 @@
         <v>13.701838731184484</v>
       </c>
       <c r="Q7" s="7"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S7" s="12"/>
+      <c r="U7" s="1"/>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="7"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -997,8 +1035,12 @@
       </c>
       <c r="P8" s="20"/>
       <c r="Q8" s="7"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S8" s="12"/>
+      <c r="U8" s="1"/>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="7"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>0</v>
       </c>
@@ -1037,8 +1079,12 @@
       </c>
       <c r="P9" s="20"/>
       <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S9" s="12"/>
+      <c r="U9" s="1"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="7"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>0</v>
       </c>
@@ -1077,8 +1123,16 @@
       </c>
       <c r="P10" s="20"/>
       <c r="Q10" s="7"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S10" s="5"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="8"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1172,7 @@
       <c r="P11" s="20"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1214,7 @@
       <c r="P12" s="20"/>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="C13" s="18"/>
       <c r="G13" s="24"/>
@@ -1188,7 +1242,7 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="25"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>7</v>
       </c>
@@ -1224,7 +1278,7 @@
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1268,7 +1322,7 @@
         <v>6.0948957860509063</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>7</v>
       </c>

</xml_diff>